<commit_message>
Code CheckIn 1 Oct
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/bin/com/mojio/xls/Suite.xlsx
+++ b/MyMojioWebsite/bin/com/mojio/xls/Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
   <si>
     <t>TSID</t>
   </si>
@@ -80,22 +80,25 @@
     <t>MyOrders</t>
   </si>
   <si>
+    <t>LocateMojio</t>
+  </si>
+  <si>
+    <t>TripHistory</t>
+  </si>
+  <si>
+    <t>Date search remains</t>
+  </si>
+  <si>
+    <t>SendFeedback</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>AdminSearch</t>
+  </si>
+  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>LocateMojio</t>
-  </si>
-  <si>
-    <t>TripHistory</t>
-  </si>
-  <si>
-    <t>Date search remains</t>
-  </si>
-  <si>
-    <t>SendFeedback</t>
-  </si>
-  <si>
-    <t>Settings</t>
   </si>
 </sst>
 </file>
@@ -217,7 +220,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C15" activeCellId="0" pane="topLeft" sqref="C15"/>
+      <selection activeCell="C21" activeCellId="0" pane="topLeft" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -385,14 +388,16 @@
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
@@ -403,10 +408,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -414,7 +419,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>4</v>
@@ -425,17 +430,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
-      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="2"/>

</xml_diff>

<commit_message>
Code Check In 8 Oct
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/bin/com/mojio/xls/Suite.xlsx
+++ b/MyMojioWebsite/bin/com/mojio/xls/Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>TSID</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>AdminSearch</t>
+  </si>
+  <si>
+    <t>AdminDashboard</t>
+  </si>
+  <si>
+    <t>ReplayEvent</t>
   </si>
   <si>
     <t>Y</t>
@@ -217,10 +223,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C21" activeCellId="0" pane="topLeft" sqref="C21"/>
+      <selection activeCell="B15" activeCellId="0" pane="topLeft" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -443,15 +449,30 @@
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
-      <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Code Check In 9 Oct
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/bin/com/mojio/xls/Suite.xlsx
+++ b/MyMojioWebsite/bin/com/mojio/xls/Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
   <si>
     <t>TSID</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>ReplayEvent</t>
+  </si>
+  <si>
+    <t>Changes where the event replay or not</t>
+  </si>
+  <si>
+    <t>ReplayReport</t>
+  </si>
+  <si>
+    <t>Changes where the report replay or not</t>
+  </si>
+  <si>
+    <t>ImportSIMs</t>
   </si>
   <si>
     <t>Y</t>
@@ -223,10 +235,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B15" activeCellId="0" pane="topLeft" sqref="B15"/>
+      <selection activeCell="B20" activeCellId="0" pane="topLeft" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -460,7 +472,9 @@
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
       </c>
@@ -469,9 +483,31 @@
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C22" s="2" t="s">
-        <v>29</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code Check In 10 Oct
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/bin/com/mojio/xls/Suite.xlsx
+++ b/MyMojioWebsite/bin/com/mojio/xls/Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="36">
   <si>
     <t>TSID</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>ImportSIMs</t>
+  </si>
+  <si>
+    <t>Testing Required</t>
+  </si>
+  <si>
+    <t>ImportMojio</t>
   </si>
   <si>
     <t>Y</t>
@@ -235,10 +241,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B20" activeCellId="0" pane="topLeft" sqref="B20"/>
+      <selection activeCell="A25" activeCellId="0" pane="topLeft" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -505,9 +511,22 @@
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C24" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>